<commit_message>
Day15 : coffee machine calculator.xlsx
</commit_message>
<xml_diff>
--- a/Day15/coffee machine calculator.xlsx
+++ b/Day15/coffee machine calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itisyijy\Desktop\100Days4Python\Day15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F750B2C-7071-4280-857A-10B7FAA4CEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D96D11-939B-4995-A1A4-3D686A70F7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3150" yWindow="1875" windowWidth="28800" windowHeight="15345" xr2:uid="{FE2C5E30-D353-4663-8481-650AB2A0D404}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{FE2C5E30-D353-4663-8481-650AB2A0D404}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,7 +484,7 @@
   <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,5 +647,6 @@
     <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>